<commit_message>
(gradescope:105/165) found that the logic o_dmem_mask, o_dmem_addr and i_dmem_rdata is totally wrong
</commit_message>
<xml_diff>
--- a/project4/all control signals.xlsx
+++ b/project4/all control signals.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/jou32/ECE552/project4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wendelin_ou/Documents/DDCA/UWM_ECE552/ECE552/project4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD9172A-EE48-A541-86A0-73F34CD3E986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31123497-71FD-FD44-A0C2-DF7A3E409242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17340" xr2:uid="{F9B3D332-2543-D640-A61B-66FC112348AC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="156">
   <si>
     <t>R</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -302,18 +302,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>4'b0001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4'b0011</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4'b1111</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>RegWrite</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -455,9 +443,6 @@
   </si>
   <si>
     <t>0</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
   <si>
     <t>ALU (alu.v)</t>
@@ -717,7 +702,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>X(1)</t>
+    <t>o_dmen_wen</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1155,13 +1140,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{997CF487-1CF8-7440-ACFC-C786920D05E2}">
-  <dimension ref="A1:X47"/>
+  <dimension ref="A1:Y47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="I36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="M19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="S50" sqref="S50"/>
+      <selection pane="bottomRight" activeCell="S15" sqref="S15:S23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1184,14 +1169,15 @@
     <col min="17" max="17" width="16.83203125" style="1" customWidth="1"/>
     <col min="18" max="18" width="8.83203125" style="1" customWidth="1"/>
     <col min="19" max="19" width="10.83203125" style="1"/>
-    <col min="20" max="20" width="13.33203125" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="10.83203125" style="1"/>
+    <col min="20" max="20" width="11.5" style="1" customWidth="1"/>
+    <col min="21" max="21" width="13.33203125" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="46" customHeight="1">
+    <row r="1" spans="1:25" ht="46" customHeight="1">
       <c r="A1" s="2"/>
       <c r="B1" s="8" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
@@ -1215,8 +1201,9 @@
       <c r="V1" s="8"/>
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
-    </row>
-    <row r="2" spans="1:24" ht="31" customHeight="1">
+      <c r="Y1" s="8"/>
+    </row>
+    <row r="2" spans="1:25" ht="31" customHeight="1">
       <c r="A2" s="6"/>
       <c r="B2" s="7"/>
       <c r="C2" s="6" t="s">
@@ -1224,7 +1211,7 @@
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
@@ -1234,7 +1221,7 @@
       <c r="K2" s="4"/>
       <c r="L2" s="2"/>
       <c r="M2" s="7" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="N2" s="7"/>
       <c r="O2" s="7"/>
@@ -1243,76 +1230,80 @@
       <c r="R2" s="4"/>
       <c r="S2" s="4"/>
       <c r="T2" s="4"/>
-      <c r="U2" s="2"/>
+      <c r="U2" s="4"/>
       <c r="V2" s="2"/>
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
-    </row>
-    <row r="3" spans="1:24" ht="32" customHeight="1">
+      <c r="Y2" s="2"/>
+    </row>
+    <row r="3" spans="1:25" ht="32" customHeight="1">
       <c r="A3" s="6"/>
       <c r="B3" s="7"/>
       <c r="C3" s="6"/>
       <c r="D3" s="3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="M3" s="6" t="s">
         <v>13</v>
       </c>
       <c r="N3" s="6"/>
       <c r="O3" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>53</v>
       </c>
       <c r="T3" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="U3" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="V3" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="V3" s="3" t="s">
+      <c r="W3" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="W3" s="3" t="s">
+      <c r="X3" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="X3" s="3"/>
-    </row>
-    <row r="4" spans="1:24" ht="32">
+      <c r="Y3" s="3"/>
+    </row>
+    <row r="4" spans="1:25" ht="32">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1323,25 +1314,25 @@
         <v>64</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>33</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>33</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="K4" s="6" t="s">
         <v>33</v>
@@ -1359,22 +1350,22 @@
         <v>33</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="Q4" s="6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="R4" s="6" t="s">
         <v>25</v>
       </c>
       <c r="S4" s="6" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="T4" s="6" t="s">
-        <v>156</v>
+        <v>33</v>
       </c>
       <c r="U4" s="6" t="s">
-        <v>33</v>
+        <v>152</v>
       </c>
       <c r="V4" s="6" t="s">
         <v>33</v>
@@ -1382,9 +1373,12 @@
       <c r="W4" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="X4" s="2"/>
-    </row>
-    <row r="5" spans="1:24" ht="16">
+      <c r="X4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y4" s="2"/>
+    </row>
+    <row r="5" spans="1:25" ht="16">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -1393,13 +1387,13 @@
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="F5" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>25</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
@@ -1413,7 +1407,7 @@
       </c>
       <c r="O5" s="6"/>
       <c r="P5" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="Q5" s="6"/>
       <c r="R5" s="6"/>
@@ -1422,9 +1416,10 @@
       <c r="U5" s="6"/>
       <c r="V5" s="6"/>
       <c r="W5" s="6"/>
-      <c r="X5" s="2"/>
-    </row>
-    <row r="6" spans="1:24" ht="16">
+      <c r="X5" s="6"/>
+      <c r="Y5" s="2"/>
+    </row>
+    <row r="6" spans="1:25" ht="16">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -1433,13 +1428,13 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>33</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
@@ -1453,7 +1448,7 @@
       </c>
       <c r="O6" s="6"/>
       <c r="P6" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="Q6" s="6"/>
       <c r="R6" s="6"/>
@@ -1462,9 +1457,10 @@
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
       <c r="W6" s="6"/>
-      <c r="X6" s="2"/>
-    </row>
-    <row r="7" spans="1:24" ht="16">
+      <c r="X6" s="6"/>
+      <c r="Y6" s="2"/>
+    </row>
+    <row r="7" spans="1:25" ht="16">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1473,27 +1469,27 @@
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>33</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
       <c r="M7" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="N7" s="2" t="s">
         <v>39</v>
       </c>
       <c r="O7" s="6"/>
       <c r="P7" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="Q7" s="6"/>
       <c r="R7" s="6"/>
@@ -1502,9 +1498,10 @@
       <c r="U7" s="6"/>
       <c r="V7" s="6"/>
       <c r="W7" s="6"/>
-      <c r="X7" s="2"/>
-    </row>
-    <row r="8" spans="1:24" ht="16">
+      <c r="X7" s="6"/>
+      <c r="Y7" s="2"/>
+    </row>
+    <row r="8" spans="1:25" ht="16">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -1513,27 +1510,27 @@
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
       <c r="M8" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="N8" s="2" t="s">
         <v>40</v>
       </c>
       <c r="O8" s="6"/>
       <c r="P8" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="Q8" s="6"/>
       <c r="R8" s="6"/>
@@ -1542,9 +1539,10 @@
       <c r="U8" s="6"/>
       <c r="V8" s="6"/>
       <c r="W8" s="6"/>
-      <c r="X8" s="2"/>
-    </row>
-    <row r="9" spans="1:24" ht="16">
+      <c r="X8" s="6"/>
+      <c r="Y8" s="2"/>
+    </row>
+    <row r="9" spans="1:25" ht="16">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -1553,13 +1551,13 @@
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
@@ -1573,7 +1571,7 @@
       </c>
       <c r="O9" s="6"/>
       <c r="P9" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="Q9" s="6"/>
       <c r="R9" s="6"/>
@@ -1582,9 +1580,10 @@
       <c r="U9" s="6"/>
       <c r="V9" s="6"/>
       <c r="W9" s="6"/>
-      <c r="X9" s="2"/>
-    </row>
-    <row r="10" spans="1:24" ht="16">
+      <c r="X9" s="6"/>
+      <c r="Y9" s="2"/>
+    </row>
+    <row r="10" spans="1:25" ht="16">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -1593,13 +1592,13 @@
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>104</v>
-      </c>
       <c r="H10" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
@@ -1613,7 +1612,7 @@
       </c>
       <c r="O10" s="6"/>
       <c r="P10" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="Q10" s="6"/>
       <c r="R10" s="6"/>
@@ -1622,9 +1621,10 @@
       <c r="U10" s="6"/>
       <c r="V10" s="6"/>
       <c r="W10" s="6"/>
-      <c r="X10" s="2"/>
-    </row>
-    <row r="11" spans="1:24" ht="16">
+      <c r="X10" s="6"/>
+      <c r="Y10" s="2"/>
+    </row>
+    <row r="11" spans="1:25" ht="16">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -1633,13 +1633,13 @@
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>25</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
@@ -1653,7 +1653,7 @@
       </c>
       <c r="O11" s="6"/>
       <c r="P11" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="Q11" s="6"/>
       <c r="R11" s="6"/>
@@ -1662,9 +1662,10 @@
       <c r="U11" s="6"/>
       <c r="V11" s="6"/>
       <c r="W11" s="6"/>
-      <c r="X11" s="2"/>
-    </row>
-    <row r="12" spans="1:24" ht="16">
+      <c r="X11" s="6"/>
+      <c r="Y11" s="2"/>
+    </row>
+    <row r="12" spans="1:25" ht="16">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -1673,7 +1674,7 @@
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>33</v>
@@ -1686,14 +1687,14 @@
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
       <c r="M12" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="N12" s="2" t="s">
         <v>45</v>
       </c>
       <c r="O12" s="6"/>
       <c r="P12" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="Q12" s="6"/>
       <c r="R12" s="6"/>
@@ -1702,9 +1703,10 @@
       <c r="U12" s="6"/>
       <c r="V12" s="6"/>
       <c r="W12" s="6"/>
-      <c r="X12" s="2"/>
-    </row>
-    <row r="13" spans="1:24" ht="16">
+      <c r="X12" s="6"/>
+      <c r="Y12" s="2"/>
+    </row>
+    <row r="13" spans="1:25" ht="16">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -1713,7 +1715,7 @@
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>33</v>
@@ -1726,14 +1728,14 @@
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
       <c r="M13" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="N13" s="2" t="s">
         <v>44</v>
       </c>
       <c r="O13" s="6"/>
       <c r="P13" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="Q13" s="6"/>
       <c r="R13" s="6"/>
@@ -1742,9 +1744,10 @@
       <c r="U13" s="6"/>
       <c r="V13" s="6"/>
       <c r="W13" s="6"/>
-      <c r="X13" s="2"/>
-    </row>
-    <row r="14" spans="1:24" ht="32">
+      <c r="X13" s="6"/>
+      <c r="Y13" s="2"/>
+    </row>
+    <row r="14" spans="1:25" ht="32">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1753,7 +1756,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -1771,8 +1774,9 @@
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
       <c r="X14" s="2"/>
-    </row>
-    <row r="15" spans="1:24" ht="16">
+      <c r="Y14" s="2"/>
+    </row>
+    <row r="15" spans="1:25" ht="16">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -1783,23 +1787,23 @@
         <v>51</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I15" s="6" t="s">
         <v>33</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="K15" s="6" t="s">
         <v>33</v>
@@ -1817,22 +1821,22 @@
         <v>33</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="Q15" s="6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="R15" s="6" t="s">
         <v>25</v>
       </c>
       <c r="S15" s="6" t="s">
-        <v>105</v>
+        <v>33</v>
       </c>
       <c r="T15" s="6" t="s">
-        <v>155</v>
+        <v>33</v>
       </c>
       <c r="U15" s="6" t="s">
-        <v>33</v>
+        <v>151</v>
       </c>
       <c r="V15" s="6" t="s">
         <v>33</v>
@@ -1840,9 +1844,12 @@
       <c r="W15" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="X15" s="2"/>
-    </row>
-    <row r="16" spans="1:24" ht="16">
+      <c r="X15" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y15" s="2"/>
+    </row>
+    <row r="16" spans="1:25" ht="16">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -1851,25 +1858,25 @@
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
       <c r="M16" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="N16" s="2" t="s">
         <v>46</v>
       </c>
       <c r="O16" s="6"/>
       <c r="P16" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="Q16" s="6"/>
       <c r="R16" s="6"/>
@@ -1878,9 +1885,10 @@
       <c r="U16" s="6"/>
       <c r="V16" s="6"/>
       <c r="W16" s="6"/>
-      <c r="X16" s="2"/>
-    </row>
-    <row r="17" spans="1:24" ht="16">
+      <c r="X16" s="6"/>
+      <c r="Y16" s="2"/>
+    </row>
+    <row r="17" spans="1:25" ht="16">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
@@ -1889,25 +1897,25 @@
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
       <c r="M17" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="N17" s="2" t="s">
         <v>39</v>
       </c>
       <c r="O17" s="6"/>
       <c r="P17" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="Q17" s="6"/>
       <c r="R17" s="6"/>
@@ -1916,9 +1924,10 @@
       <c r="U17" s="6"/>
       <c r="V17" s="6"/>
       <c r="W17" s="6"/>
-      <c r="X17" s="2"/>
-    </row>
-    <row r="18" spans="1:24" ht="16">
+      <c r="X17" s="6"/>
+      <c r="Y17" s="2"/>
+    </row>
+    <row r="18" spans="1:25" ht="16">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
@@ -1927,25 +1936,25 @@
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
       <c r="M18" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="N18" s="2" t="s">
         <v>40</v>
       </c>
       <c r="O18" s="6"/>
       <c r="P18" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="Q18" s="6"/>
       <c r="R18" s="6"/>
@@ -1954,9 +1963,10 @@
       <c r="U18" s="6"/>
       <c r="V18" s="6"/>
       <c r="W18" s="6"/>
-      <c r="X18" s="2"/>
-    </row>
-    <row r="19" spans="1:24" ht="16">
+      <c r="X18" s="6"/>
+      <c r="Y18" s="2"/>
+    </row>
+    <row r="19" spans="1:25" ht="16">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
@@ -1965,11 +1975,11 @@
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
@@ -1983,7 +1993,7 @@
       </c>
       <c r="O19" s="6"/>
       <c r="P19" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="Q19" s="6"/>
       <c r="R19" s="6"/>
@@ -1992,9 +2002,10 @@
       <c r="U19" s="6"/>
       <c r="V19" s="6"/>
       <c r="W19" s="6"/>
-      <c r="X19" s="2"/>
-    </row>
-    <row r="20" spans="1:24" ht="16">
+      <c r="X19" s="6"/>
+      <c r="Y19" s="2"/>
+    </row>
+    <row r="20" spans="1:25" ht="16">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
@@ -2003,27 +2014,27 @@
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>33</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
       <c r="M20" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="N20" s="2" t="s">
         <v>48</v>
       </c>
       <c r="O20" s="6"/>
       <c r="P20" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="Q20" s="6"/>
       <c r="R20" s="6"/>
@@ -2032,9 +2043,10 @@
       <c r="U20" s="6"/>
       <c r="V20" s="6"/>
       <c r="W20" s="6"/>
-      <c r="X20" s="2"/>
-    </row>
-    <row r="21" spans="1:24" ht="16">
+      <c r="X20" s="6"/>
+      <c r="Y20" s="2"/>
+    </row>
+    <row r="21" spans="1:25" ht="16">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
@@ -2043,27 +2055,27 @@
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>25</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
       <c r="M21" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="N21" s="2" t="s">
         <v>50</v>
       </c>
       <c r="O21" s="6"/>
       <c r="P21" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="Q21" s="6"/>
       <c r="R21" s="6"/>
@@ -2072,9 +2084,10 @@
       <c r="U21" s="6"/>
       <c r="V21" s="6"/>
       <c r="W21" s="6"/>
-      <c r="X21" s="2"/>
-    </row>
-    <row r="22" spans="1:24" ht="16">
+      <c r="X21" s="6"/>
+      <c r="Y21" s="2"/>
+    </row>
+    <row r="22" spans="1:25" ht="16">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
@@ -2083,7 +2096,7 @@
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="F22" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2" t="s">
@@ -2094,14 +2107,14 @@
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
       <c r="M22" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="N22" s="2" t="s">
         <v>45</v>
       </c>
       <c r="O22" s="6"/>
       <c r="P22" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
@@ -2110,9 +2123,10 @@
       <c r="U22" s="6"/>
       <c r="V22" s="6"/>
       <c r="W22" s="6"/>
-      <c r="X22" s="2"/>
-    </row>
-    <row r="23" spans="1:24" ht="16">
+      <c r="X22" s="6"/>
+      <c r="Y22" s="2"/>
+    </row>
+    <row r="23" spans="1:25" ht="16">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
@@ -2121,7 +2135,7 @@
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2" t="s">
@@ -2132,14 +2146,14 @@
       <c r="K23" s="6"/>
       <c r="L23" s="6"/>
       <c r="M23" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="N23" s="2" t="s">
         <v>44</v>
       </c>
       <c r="O23" s="6"/>
       <c r="P23" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="Q23" s="6"/>
       <c r="R23" s="6"/>
@@ -2148,9 +2162,10 @@
       <c r="U23" s="6"/>
       <c r="V23" s="6"/>
       <c r="W23" s="6"/>
-      <c r="X23" s="2"/>
-    </row>
-    <row r="24" spans="1:24" ht="32">
+      <c r="X23" s="6"/>
+      <c r="Y23" s="2"/>
+    </row>
+    <row r="24" spans="1:25" ht="32">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -2159,7 +2174,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -2177,8 +2192,9 @@
       <c r="V24" s="2"/>
       <c r="W24" s="2"/>
       <c r="X24" s="2"/>
-    </row>
-    <row r="25" spans="1:24" ht="16">
+      <c r="Y24" s="2"/>
+    </row>
+    <row r="25" spans="1:25" ht="16">
       <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
@@ -2189,23 +2205,23 @@
         <v>52</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>55</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I25" s="6" t="s">
         <v>33</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="K25" s="6" t="s">
         <v>33</v>
@@ -2223,10 +2239,10 @@
         <v>33</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="Q25" s="6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="R25" s="6" t="s">
         <v>33</v>
@@ -2235,20 +2251,23 @@
         <v>25</v>
       </c>
       <c r="T25" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="U25" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="U25" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="V25" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="V25" s="6" t="s">
-        <v>33</v>
-      </c>
       <c r="W25" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="X25" s="2"/>
-    </row>
-    <row r="26" spans="1:24" ht="16">
+      <c r="X25" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y25" s="2"/>
+    </row>
+    <row r="26" spans="1:25" ht="16">
       <c r="A26" s="2" t="s">
         <v>27</v>
       </c>
@@ -2257,11 +2276,11 @@
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
@@ -2275,18 +2294,21 @@
       </c>
       <c r="O26" s="6"/>
       <c r="P26" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="Q26" s="6"/>
       <c r="R26" s="6"/>
       <c r="S26" s="6"/>
       <c r="T26" s="6"/>
-      <c r="U26" s="6"/>
+      <c r="U26" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="V26" s="6"/>
       <c r="W26" s="6"/>
-      <c r="X26" s="2"/>
-    </row>
-    <row r="27" spans="1:24" ht="16">
+      <c r="X26" s="6"/>
+      <c r="Y26" s="2"/>
+    </row>
+    <row r="27" spans="1:25" ht="16">
       <c r="A27" s="2" t="s">
         <v>28</v>
       </c>
@@ -2295,11 +2317,11 @@
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
       <c r="F27" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
@@ -2313,18 +2335,21 @@
       </c>
       <c r="O27" s="6"/>
       <c r="P27" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="Q27" s="6"/>
       <c r="R27" s="6"/>
       <c r="S27" s="6"/>
       <c r="T27" s="6"/>
-      <c r="U27" s="6"/>
+      <c r="U27" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="V27" s="6"/>
       <c r="W27" s="6"/>
-      <c r="X27" s="2"/>
-    </row>
-    <row r="28" spans="1:24" ht="16">
+      <c r="X27" s="6"/>
+      <c r="Y27" s="2"/>
+    </row>
+    <row r="28" spans="1:25" ht="16">
       <c r="A28" s="2" t="s">
         <v>29</v>
       </c>
@@ -2333,11 +2358,11 @@
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
       <c r="F28" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
@@ -2351,18 +2376,21 @@
       </c>
       <c r="O28" s="6"/>
       <c r="P28" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="Q28" s="6"/>
       <c r="R28" s="6"/>
       <c r="S28" s="6"/>
       <c r="T28" s="6"/>
-      <c r="U28" s="6"/>
+      <c r="U28" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="V28" s="6"/>
       <c r="W28" s="6"/>
-      <c r="X28" s="2"/>
-    </row>
-    <row r="29" spans="1:24" ht="16">
+      <c r="X28" s="6"/>
+      <c r="Y28" s="2"/>
+    </row>
+    <row r="29" spans="1:25" ht="16">
       <c r="A29" s="2" t="s">
         <v>30</v>
       </c>
@@ -2371,11 +2399,11 @@
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
       <c r="F29" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
@@ -2389,18 +2417,21 @@
       </c>
       <c r="O29" s="6"/>
       <c r="P29" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="Q29" s="6"/>
       <c r="R29" s="6"/>
       <c r="S29" s="6"/>
       <c r="T29" s="6"/>
-      <c r="U29" s="6"/>
+      <c r="U29" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="V29" s="6"/>
       <c r="W29" s="6"/>
-      <c r="X29" s="2"/>
-    </row>
-    <row r="30" spans="1:24" ht="16">
+      <c r="X29" s="6"/>
+      <c r="Y29" s="2"/>
+    </row>
+    <row r="30" spans="1:25" ht="16">
       <c r="A30" s="2" t="s">
         <v>61</v>
       </c>
@@ -2411,21 +2442,21 @@
         <v>60</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E30" s="6"/>
       <c r="F30" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="I30" s="6" t="s">
         <v>33</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="K30" s="6" t="s">
         <v>33</v>
@@ -2443,10 +2474,10 @@
         <v>33</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="Q30" s="6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="R30" s="6" t="s">
         <v>33</v>
@@ -2454,21 +2485,24 @@
       <c r="S30" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="T30" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="U30" s="6" t="s">
+      <c r="T30" s="6" t="s">
         <v>25</v>
       </c>
+      <c r="U30" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="V30" s="6" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="W30" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="X30" s="2"/>
-    </row>
-    <row r="31" spans="1:24" ht="16">
+      <c r="X30" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y30" s="2"/>
+    </row>
+    <row r="31" spans="1:25" ht="16">
       <c r="A31" s="2" t="s">
         <v>62</v>
       </c>
@@ -2477,11 +2511,11 @@
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
       <c r="F31" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
@@ -2495,20 +2529,21 @@
       </c>
       <c r="O31" s="6"/>
       <c r="P31" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="Q31" s="6"/>
       <c r="R31" s="6"/>
       <c r="S31" s="6"/>
-      <c r="T31" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="U31" s="6"/>
+      <c r="T31" s="6"/>
+      <c r="U31" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="V31" s="6"/>
       <c r="W31" s="6"/>
-      <c r="X31" s="2"/>
-    </row>
-    <row r="32" spans="1:24" ht="16">
+      <c r="X31" s="6"/>
+      <c r="Y31" s="2"/>
+    </row>
+    <row r="32" spans="1:25" ht="16">
       <c r="A32" s="2" t="s">
         <v>63</v>
       </c>
@@ -2517,11 +2552,11 @@
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
       <c r="F32" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="I32" s="6"/>
       <c r="J32" s="6"/>
@@ -2535,20 +2570,21 @@
       </c>
       <c r="O32" s="6"/>
       <c r="P32" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="Q32" s="6"/>
       <c r="R32" s="6"/>
       <c r="S32" s="6"/>
-      <c r="T32" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="U32" s="6"/>
+      <c r="T32" s="6"/>
+      <c r="U32" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="V32" s="6"/>
       <c r="W32" s="6"/>
-      <c r="X32" s="2"/>
-    </row>
-    <row r="33" spans="1:24" ht="32">
+      <c r="X32" s="6"/>
+      <c r="Y32" s="2"/>
+    </row>
+    <row r="33" spans="1:25" ht="32">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -2557,7 +2593,7 @@
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
@@ -2575,35 +2611,36 @@
       <c r="V33" s="2"/>
       <c r="W33" s="2"/>
       <c r="X33" s="2"/>
-    </row>
-    <row r="34" spans="1:24" ht="16">
+      <c r="Y33" s="2"/>
+    </row>
+    <row r="34" spans="1:25" ht="16">
       <c r="A34" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="I34" s="2" t="s">
         <v>33</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="K34" s="6" t="s">
         <v>33</v>
@@ -2612,7 +2649,7 @@
         <v>33</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="N34" s="2" t="s">
         <v>50</v>
@@ -2621,45 +2658,48 @@
         <v>33</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="Q34" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="R34" s="6" t="s">
         <v>33</v>
       </c>
       <c r="S34" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="T34" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="U34" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="V34" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="W34" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="T34" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="U34" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="V34" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="W34" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="X34" s="2"/>
-    </row>
-    <row r="35" spans="1:24" ht="16">
+      <c r="X34" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y34" s="2"/>
+    </row>
+    <row r="35" spans="1:25" ht="16">
       <c r="A35" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
       <c r="F35" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G35" s="2"/>
       <c r="H35" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="I35" s="2" t="s">
         <v>25</v>
@@ -2668,7 +2708,7 @@
       <c r="K35" s="6"/>
       <c r="L35" s="6"/>
       <c r="M35" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="N35" s="2" t="s">
         <v>50</v>
@@ -2677,10 +2717,10 @@
         <v>25</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="Q35" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="R35" s="6"/>
       <c r="S35" s="6"/>
@@ -2688,22 +2728,23 @@
       <c r="U35" s="6"/>
       <c r="V35" s="6"/>
       <c r="W35" s="6"/>
-      <c r="X35" s="2"/>
-    </row>
-    <row r="36" spans="1:24" ht="16">
+      <c r="X35" s="6"/>
+      <c r="Y35" s="2"/>
+    </row>
+    <row r="36" spans="1:25" ht="16">
       <c r="A36" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
       <c r="F36" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G36" s="2"/>
       <c r="H36" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="I36" s="2" t="s">
         <v>33</v>
@@ -2712,7 +2753,7 @@
       <c r="K36" s="6"/>
       <c r="L36" s="6"/>
       <c r="M36" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="N36" s="2" t="s">
         <v>39</v>
@@ -2721,10 +2762,10 @@
         <v>33</v>
       </c>
       <c r="P36" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="Q36" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="R36" s="6"/>
       <c r="S36" s="6"/>
@@ -2732,22 +2773,23 @@
       <c r="U36" s="6"/>
       <c r="V36" s="6"/>
       <c r="W36" s="6"/>
-      <c r="X36" s="2"/>
-    </row>
-    <row r="37" spans="1:24" ht="16">
+      <c r="X36" s="6"/>
+      <c r="Y36" s="2"/>
+    </row>
+    <row r="37" spans="1:25" ht="16">
       <c r="A37" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G37" s="2"/>
       <c r="H37" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="I37" s="2" t="s">
         <v>33</v>
@@ -2756,19 +2798,19 @@
       <c r="K37" s="6"/>
       <c r="L37" s="6"/>
       <c r="M37" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="N37" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="O37" s="2" t="s">
         <v>33</v>
       </c>
       <c r="P37" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="Q37" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="R37" s="6"/>
       <c r="S37" s="6"/>
@@ -2776,22 +2818,23 @@
       <c r="U37" s="6"/>
       <c r="V37" s="6"/>
       <c r="W37" s="6"/>
-      <c r="X37" s="2"/>
-    </row>
-    <row r="38" spans="1:24" ht="16">
+      <c r="X37" s="6"/>
+      <c r="Y37" s="2"/>
+    </row>
+    <row r="38" spans="1:25" ht="16">
       <c r="A38" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I38" s="2" t="s">
         <v>33</v>
@@ -2800,7 +2843,7 @@
       <c r="K38" s="6"/>
       <c r="L38" s="6"/>
       <c r="M38" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="N38" s="2" t="s">
         <v>40</v>
@@ -2809,10 +2852,10 @@
         <v>33</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="Q38" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="R38" s="6"/>
       <c r="S38" s="6"/>
@@ -2820,22 +2863,23 @@
       <c r="U38" s="6"/>
       <c r="V38" s="6"/>
       <c r="W38" s="6"/>
-      <c r="X38" s="2"/>
-    </row>
-    <row r="39" spans="1:24" ht="16">
+      <c r="X38" s="6"/>
+      <c r="Y38" s="2"/>
+    </row>
+    <row r="39" spans="1:25" ht="16">
       <c r="A39" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="I39" s="2" t="s">
         <v>33</v>
@@ -2844,7 +2888,7 @@
       <c r="K39" s="6"/>
       <c r="L39" s="6"/>
       <c r="M39" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="N39" s="2" t="s">
         <v>48</v>
@@ -2853,10 +2897,10 @@
         <v>33</v>
       </c>
       <c r="P39" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="Q39" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="R39" s="6"/>
       <c r="S39" s="6"/>
@@ -2864,9 +2908,10 @@
       <c r="U39" s="6"/>
       <c r="V39" s="6"/>
       <c r="W39" s="6"/>
-      <c r="X39" s="2"/>
-    </row>
-    <row r="40" spans="1:24" ht="32">
+      <c r="X39" s="6"/>
+      <c r="Y39" s="2"/>
+    </row>
+    <row r="40" spans="1:25" ht="32">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -2875,7 +2920,7 @@
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
@@ -2893,19 +2938,20 @@
       <c r="V40" s="2"/>
       <c r="W40" s="2"/>
       <c r="X40" s="2"/>
-    </row>
-    <row r="41" spans="1:24" ht="32" customHeight="1">
+      <c r="Y40" s="2"/>
+    </row>
+    <row r="41" spans="1:25" ht="32" customHeight="1">
       <c r="A41" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>55</v>
@@ -2913,7 +2959,7 @@
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I41" s="2" t="s">
         <v>33</v>
@@ -2937,22 +2983,22 @@
         <v>33</v>
       </c>
       <c r="P41" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="Q41" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="R41" s="6" t="s">
         <v>25</v>
       </c>
       <c r="S41" s="6" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="T41" s="6" t="s">
-        <v>155</v>
+        <v>33</v>
       </c>
       <c r="U41" s="6" t="s">
-        <v>33</v>
+        <v>151</v>
       </c>
       <c r="V41" s="6" t="s">
         <v>33</v>
@@ -2960,25 +3006,28 @@
       <c r="W41" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="X41" s="2"/>
-    </row>
-    <row r="42" spans="1:24" ht="32" customHeight="1">
+      <c r="X41" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y41" s="2"/>
+    </row>
+    <row r="42" spans="1:25" ht="32" customHeight="1">
       <c r="A42" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B42" s="6"/>
       <c r="C42" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="J42" s="2" t="s">
         <v>33</v>
@@ -2992,13 +3041,13 @@
         <v>33</v>
       </c>
       <c r="O42" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="P42" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="Q42" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="R42" s="6"/>
       <c r="S42" s="6"/>
@@ -3006,20 +3055,21 @@
       <c r="U42" s="6"/>
       <c r="V42" s="6"/>
       <c r="W42" s="6"/>
-      <c r="X42" s="2"/>
-    </row>
-    <row r="43" spans="1:24" ht="16">
+      <c r="X42" s="6"/>
+      <c r="Y42" s="2"/>
+    </row>
+    <row r="43" spans="1:25" ht="16">
       <c r="A43" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>55</v>
@@ -3027,10 +3077,10 @@
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="J43" s="2" t="s">
         <v>33</v>
@@ -3048,56 +3098,59 @@
         <v>33</v>
       </c>
       <c r="O43" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="P43" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="Q43" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="R43" s="6"/>
       <c r="S43" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="T43" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="U43" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="V43" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="W43" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="X43" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="T43" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="U43" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="V43" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="W43" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="X43" s="2"/>
-    </row>
-    <row r="44" spans="1:24" ht="16">
+      <c r="Y43" s="2"/>
+    </row>
+    <row r="44" spans="1:25" ht="16">
       <c r="A44" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C44" s="6"/>
       <c r="D44" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E44" s="6"/>
       <c r="F44" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G44" s="2"/>
       <c r="H44" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="K44" s="2" t="s">
         <v>33</v>
@@ -3112,13 +3165,13 @@
         <v>33</v>
       </c>
       <c r="O44" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="P44" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="Q44" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="R44" s="6"/>
       <c r="S44" s="6"/>
@@ -3126,9 +3179,10 @@
       <c r="U44" s="6"/>
       <c r="V44" s="6"/>
       <c r="W44" s="6"/>
-      <c r="X44" s="2"/>
-    </row>
-    <row r="45" spans="1:24">
+      <c r="X44" s="6"/>
+      <c r="Y44" s="2"/>
+    </row>
+    <row r="45" spans="1:25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -3153,33 +3207,34 @@
       <c r="V45" s="2"/>
       <c r="W45" s="2"/>
       <c r="X45" s="2"/>
-    </row>
-    <row r="46" spans="1:24" ht="15" customHeight="1">
+      <c r="Y45" s="2"/>
+    </row>
+    <row r="46" spans="1:25" ht="15" customHeight="1">
       <c r="A46" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>55</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G46" s="2"/>
       <c r="H46" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I46" s="2" t="s">
         <v>33</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="K46" s="2" t="s">
         <v>33</v>
@@ -3197,70 +3252,64 @@
         <v>33</v>
       </c>
       <c r="P46" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="Q46" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="R46" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="S46" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="T46" s="2"/>
+        <v>33</v>
+      </c>
+      <c r="T46" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="U46" s="2"/>
       <c r="V46" s="2"/>
       <c r="W46" s="2"/>
       <c r="X46" s="2"/>
-    </row>
-    <row r="47" spans="1:24">
+      <c r="Y46" s="2"/>
+    </row>
+    <row r="47" spans="1:25">
       <c r="E47" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="100">
-    <mergeCell ref="B34:B39"/>
-    <mergeCell ref="C34:C39"/>
-    <mergeCell ref="D34:D39"/>
-    <mergeCell ref="L34:L39"/>
-    <mergeCell ref="W34:W39"/>
-    <mergeCell ref="V34:V39"/>
-    <mergeCell ref="E34:E39"/>
-    <mergeCell ref="K34:K39"/>
-    <mergeCell ref="R34:R39"/>
-    <mergeCell ref="J34:J39"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="W41:W42"/>
-    <mergeCell ref="R41:R44"/>
-    <mergeCell ref="L41:L42"/>
-    <mergeCell ref="V41:V42"/>
+  <mergeCells count="106">
     <mergeCell ref="W43:W44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="S30:S32"/>
-    <mergeCell ref="S25:S29"/>
-    <mergeCell ref="E4:E13"/>
-    <mergeCell ref="L4:L13"/>
-    <mergeCell ref="K30:K32"/>
-    <mergeCell ref="L30:L32"/>
-    <mergeCell ref="S4:S13"/>
-    <mergeCell ref="R4:R13"/>
-    <mergeCell ref="R15:R23"/>
-    <mergeCell ref="S15:S23"/>
-    <mergeCell ref="O30:O32"/>
-    <mergeCell ref="I4:I13"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="C25:C29"/>
-    <mergeCell ref="E15:E23"/>
-    <mergeCell ref="D4:D13"/>
-    <mergeCell ref="B4:B13"/>
-    <mergeCell ref="C4:C13"/>
-    <mergeCell ref="C15:C23"/>
-    <mergeCell ref="B1:X1"/>
+    <mergeCell ref="T4:T13"/>
+    <mergeCell ref="T15:T23"/>
+    <mergeCell ref="T25:T29"/>
+    <mergeCell ref="T30:T32"/>
+    <mergeCell ref="T34:T39"/>
+    <mergeCell ref="T41:T42"/>
+    <mergeCell ref="T43:T44"/>
+    <mergeCell ref="V30:V32"/>
+    <mergeCell ref="W25:W29"/>
+    <mergeCell ref="X25:X29"/>
+    <mergeCell ref="W30:W32"/>
+    <mergeCell ref="X30:X32"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="K41:K42"/>
+    <mergeCell ref="Q4:Q13"/>
+    <mergeCell ref="Q15:Q23"/>
+    <mergeCell ref="Q25:Q29"/>
+    <mergeCell ref="Q30:Q32"/>
+    <mergeCell ref="X4:X13"/>
+    <mergeCell ref="O4:O13"/>
+    <mergeCell ref="O15:O23"/>
+    <mergeCell ref="O25:O29"/>
+    <mergeCell ref="W15:W23"/>
+    <mergeCell ref="X15:X23"/>
+    <mergeCell ref="V4:V13"/>
+    <mergeCell ref="V15:V23"/>
+    <mergeCell ref="V25:V29"/>
+    <mergeCell ref="W4:W13"/>
+    <mergeCell ref="U4:U13"/>
+    <mergeCell ref="U15:U23"/>
+    <mergeCell ref="B1:Y1"/>
     <mergeCell ref="E25:E32"/>
     <mergeCell ref="R25:R29"/>
     <mergeCell ref="R30:R32"/>
@@ -3276,55 +3325,70 @@
     <mergeCell ref="K4:K13"/>
     <mergeCell ref="C30:C32"/>
     <mergeCell ref="D30:D32"/>
-    <mergeCell ref="W4:W13"/>
-    <mergeCell ref="O4:O13"/>
-    <mergeCell ref="O15:O23"/>
-    <mergeCell ref="O25:O29"/>
-    <mergeCell ref="V15:V23"/>
-    <mergeCell ref="W15:W23"/>
-    <mergeCell ref="U4:U13"/>
-    <mergeCell ref="U15:U23"/>
-    <mergeCell ref="T25:T29"/>
-    <mergeCell ref="U25:U29"/>
-    <mergeCell ref="V4:V13"/>
-    <mergeCell ref="T4:T13"/>
-    <mergeCell ref="T15:T23"/>
-    <mergeCell ref="I15:I23"/>
-    <mergeCell ref="I25:I29"/>
-    <mergeCell ref="I30:I32"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C25:C29"/>
+    <mergeCell ref="E15:E23"/>
+    <mergeCell ref="D4:D13"/>
+    <mergeCell ref="B4:B13"/>
+    <mergeCell ref="C4:C13"/>
+    <mergeCell ref="C15:C23"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="B15:B23"/>
     <mergeCell ref="B25:B29"/>
     <mergeCell ref="D15:D23"/>
     <mergeCell ref="D25:D29"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="K41:K42"/>
-    <mergeCell ref="Q4:Q13"/>
-    <mergeCell ref="Q15:Q23"/>
-    <mergeCell ref="Q25:Q29"/>
-    <mergeCell ref="Q30:Q32"/>
-    <mergeCell ref="U30:U32"/>
-    <mergeCell ref="V25:V29"/>
-    <mergeCell ref="W25:W29"/>
-    <mergeCell ref="V30:V32"/>
-    <mergeCell ref="W30:W32"/>
+    <mergeCell ref="S30:S32"/>
+    <mergeCell ref="S25:S29"/>
+    <mergeCell ref="E4:E13"/>
+    <mergeCell ref="L4:L13"/>
+    <mergeCell ref="K30:K32"/>
+    <mergeCell ref="L30:L32"/>
+    <mergeCell ref="S4:S13"/>
+    <mergeCell ref="R4:R13"/>
+    <mergeCell ref="R15:R23"/>
+    <mergeCell ref="S15:S23"/>
+    <mergeCell ref="O30:O32"/>
+    <mergeCell ref="I4:I13"/>
+    <mergeCell ref="I15:I23"/>
+    <mergeCell ref="I25:I29"/>
+    <mergeCell ref="I30:I32"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="X41:X42"/>
+    <mergeCell ref="R41:R44"/>
+    <mergeCell ref="L41:L42"/>
+    <mergeCell ref="W41:W42"/>
+    <mergeCell ref="X43:X44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="S41:S42"/>
+    <mergeCell ref="U41:U42"/>
+    <mergeCell ref="S43:S44"/>
+    <mergeCell ref="U43:U44"/>
+    <mergeCell ref="V41:V42"/>
+    <mergeCell ref="V43:V44"/>
+    <mergeCell ref="B34:B39"/>
+    <mergeCell ref="C34:C39"/>
+    <mergeCell ref="D34:D39"/>
+    <mergeCell ref="L34:L39"/>
+    <mergeCell ref="X34:X39"/>
+    <mergeCell ref="W34:W39"/>
+    <mergeCell ref="E34:E39"/>
+    <mergeCell ref="K34:K39"/>
+    <mergeCell ref="R34:R39"/>
+    <mergeCell ref="J34:J39"/>
     <mergeCell ref="S34:S39"/>
-    <mergeCell ref="T34:T39"/>
     <mergeCell ref="U34:U39"/>
-    <mergeCell ref="S41:S42"/>
-    <mergeCell ref="T41:T42"/>
-    <mergeCell ref="S43:S44"/>
-    <mergeCell ref="T43:T44"/>
-    <mergeCell ref="U41:U42"/>
-    <mergeCell ref="U43:U44"/>
-    <mergeCell ref="V43:V44"/>
+    <mergeCell ref="V34:V39"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <ignoredErrors>
-    <ignoredError sqref="A44:C44 A43:C43 A3:C3 X2 K3:M3 A5:D5 L44:N44 B2:C2 R41 R44 R43 A7:D7 A6:D6 R4 N16 A15:C15 A8:D8 A4:C4 K4:N4 K5:N5 K6:L6 K7:L7 K8:L8 A9:D9 K9:N9 A10:D10 K10:L10 A11:D11 K11:N11 A12:D12 K12:L12 A13:D13 K13:L13 K15:N15 A16:A23 M17:N19 A25:A29 K2:L2 N2 G11 G5 A42:D42 L38 L37 L42 L39 N6:N8 N12:N13 A30:C30 A31:D31 A32:D32 G30:G32 R25:S25 S30:T30 S32:T32 A34:C34 A35:D35 A36:D36 R2:V3 A37:D39 G35:G39 Q2 L35:L36 A41:C41 F41:G43 L34 S26:S27 S28:S29 S31:T31 X34:X39 L41 M25:N32 E5 E7 E6 E20:E21 E16 E22 E23 E15 E8 E9 E10 E11 E12 E13 E17 E18 E19 E26:E29 V41 U4 N20:N23 X4:X13 X15:X23 N10 C20:C21 C16 C22 C23 C17 C18 C19 C26:C29 C25 V34:V39 X25:X32 R42 U41 G44" numberStoredAsText="1"/>
+    <ignoredError sqref="A44:C44 A43:C43 A3:C3 Y2 K3:M3 A5:D5 L44:N44 B2:C2 R41 R44 R43 A7:D7 A6:D6 R4 N16 A15:C15 A8:D8 A4:C4 K4:N4 K5:N5 K6:L6 K7:L7 K8:L8 A9:D9 K9:N9 A10:D10 K10:L10 A11:D11 K11:N11 A12:D12 K12:L12 A13:D13 K13:L13 K15:N15 A16:A23 M17:N19 A25:A29 K2:L2 N2 G11 G5 A42:D42 L38 L37 L42 L39 N6:N8 N12:N13 A30:C30 A31:D31 A32:D32 G30:G32 R25:S25 A34:C34 A35:D35 A36:D36 U2:W2 A37:D39 G35:G39 Q2 L35:L36 A41:C41 F41:G43 L34 S26:S27 S28:S29 Y34:Y39 L41 M25:N32 E5 E7 E6 E20:E21 E16 E22 E23 E15 E8 E9 E10 E11 E12 E13 E17 E18 E19 E26:E29 W41 V4 N20:N23 Y4:Y13 Y15:Y23 N10 C20:C21 C16 C22 C23 C17 C18 C19 C26:C29 C25 W34:W39 Y25:Y32 R42 V41 G44 S31 R2:S3 S32 S30 V3:W3" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>